<commit_message>
Adding mast wire fairing Adding mast wire fairing
</commit_message>
<xml_diff>
--- a/Electric Kitefoil BOM.xlsx
+++ b/Electric Kitefoil BOM.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,87 +21,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="108">
-  <si>
-    <t xml:space="preserve">Part</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Part number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kitefoil Thruster Assy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSS56104 500kV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brushless Motor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ebay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.ebay.com/itm/SSS-56104-500KV-6-pole-brushless-motor-/152600709580</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gearbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neugart PLE40-008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.ebay.com/itm/NEUGART-PLE-40-GEARHEAD-REDUCER-FREE-SHIP-/251343315130?hash=item3a853aa0ba:g:bAIAAOxy0QBSPPOQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BHCS M4X0.7X6MM 18-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mcmaster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92095A188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R005</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="110">
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Part number</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>Mass kg</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>R001</t>
+  </si>
+  <si>
+    <t>Kitefoil Thruster Assy</t>
+  </si>
+  <si>
+    <t>R002</t>
+  </si>
+  <si>
+    <t>SSS56104 500kV</t>
+  </si>
+  <si>
+    <t>Brushless Motor</t>
+  </si>
+  <si>
+    <t>Ebay</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/SSS-56104-500KV-6-pole-brushless-motor-/152600709580</t>
+  </si>
+  <si>
+    <t>R003</t>
+  </si>
+  <si>
+    <t>gearbox</t>
+  </si>
+  <si>
+    <t>Neugart PLE40-008</t>
+  </si>
+  <si>
+    <t>http://www.ebay.com/itm/NEUGART-PLE-40-GEARHEAD-REDUCER-FREE-SHIP-/251343315130?hash=item3a853aa0ba:g:bAIAAOxy0QBSPPOQ</t>
+  </si>
+  <si>
+    <t>R004</t>
+  </si>
+  <si>
+    <t>BHCS M4X0.7X6MM 18-8</t>
+  </si>
+  <si>
+    <t>Mcmaster</t>
+  </si>
+  <si>
+    <t>92095A188</t>
+  </si>
+  <si>
+    <t>R005</t>
   </si>
   <si>
     <r>
@@ -113,7 +112,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">FHCS M4 X 0.7</t>
+      <t>FHCS M4 X 0.7</t>
     </r>
     <r>
       <rPr>
@@ -136,254 +135,257 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">92125A188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O-Ring 1/8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.25 OD 2.0ID, 1/8in Dash 226 Buna-N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9452K64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mcmaster.com/#9452k64/=18ufglf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hobbywing Seaking HV V3 130A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.4Ghz Eskate Remote - with waterproof modification?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ali-Express</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.aliexpress.com/item/2-4Ghz-Remote-Controller-With-Receiver-Universal-for-All-ESC-Electric-Skateboard-Longboard-Skate-Board-Scooter/32817830821.html?spm=a2g0s.9042311.0.0.bTzUPk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Battery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tattu Plus 6S 16000mAh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pelican Case 1200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8mm Shaft L= 65mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8mm ground shaft, 65MMLength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8MM to 10MM Shaft Coupler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uxcell® 8mm to 10mm Elastic Shaft Coupling 30mm Length 25mm Diameter Motor Coupler Aluminum Alloy Joint Connector for DIY Encoder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a16121900ux0451</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.ca/dp/B06X9XSNQ2/ref=pe_3034960_233709270_TE_item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oil Seal Bushing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bearing 8MM ID 11MM OD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6153K51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thrust Bearing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5909K11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thrust Bearing Washer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5909K71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Propeller shaft attachment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TBD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8, 10, or 12 AWG wire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epoxy or Acrylic glue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4 X 10MM ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mount gearbox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M3 X 10MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oil seal cap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M4 X 25MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nose cone to front cap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M5 X 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nose cone foil mount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M5 NUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTS Parts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">motor tube</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.5IN OD 0.125IN WALL, 12IN Length 6061 T6 Tube</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Online Metals, Mcmaster, Metal Supermarkets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">motor_gear_adapter_A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6061-T6 0.125IN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">motor_gear_adapter_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">front_cap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6061-T6 2.5IN ROUND BAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gear_mount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shaft_cap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nose_cone_A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3D PRINT PLA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nose_cone_B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propeller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reverse bushing</t>
+    <t>92125A188</t>
+  </si>
+  <si>
+    <t>R006</t>
+  </si>
+  <si>
+    <t>O-Ring 1/8</t>
+  </si>
+  <si>
+    <t>2.25 OD 2.0ID, 1/8in Dash 226 Buna-N</t>
+  </si>
+  <si>
+    <t>9452K64</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#9452k64/=18ufglf</t>
+  </si>
+  <si>
+    <t>R007</t>
+  </si>
+  <si>
+    <t>ESC</t>
+  </si>
+  <si>
+    <t>Hobbywing Seaking HV V3 130A</t>
+  </si>
+  <si>
+    <t>R008</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>2.4Ghz Eskate Remote - with waterproof modification?</t>
+  </si>
+  <si>
+    <t>Ali-Express</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/2-4Ghz-Remote-Controller-With-Receiver-Universal-for-All-ESC-Electric-Skateboard-Longboard-Skate-Board-Scooter/32817830821.html?spm=a2g0s.9042311.0.0.bTzUPk</t>
+  </si>
+  <si>
+    <t>R009</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Tattu Plus 6S 16000mAh</t>
+  </si>
+  <si>
+    <t>R010</t>
+  </si>
+  <si>
+    <t>Pelican Case 1200</t>
+  </si>
+  <si>
+    <t>MEC</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>R011</t>
+  </si>
+  <si>
+    <t>8mm Shaft L= 65mm</t>
+  </si>
+  <si>
+    <t>8mm ground shaft, 65MMLength</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>R012</t>
+  </si>
+  <si>
+    <t>8MM to 10MM Shaft Coupler</t>
+  </si>
+  <si>
+    <t>uxcell® 8mm to 10mm Elastic Shaft Coupling 30mm Length 25mm Diameter Motor Coupler Aluminum Alloy Joint Connector for DIY Encoder</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>a16121900ux0451</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/dp/B06X9XSNQ2/ref=pe_3034960_233709270_TE_item</t>
+  </si>
+  <si>
+    <t>R013</t>
+  </si>
+  <si>
+    <t>Oil Seal Bushing</t>
+  </si>
+  <si>
+    <t>R014</t>
+  </si>
+  <si>
+    <t>Bearing 8MM ID 11MM OD</t>
+  </si>
+  <si>
+    <t>6153K51</t>
+  </si>
+  <si>
+    <t>R015</t>
+  </si>
+  <si>
+    <t>Thrust Bearing</t>
+  </si>
+  <si>
+    <t>5909K11</t>
+  </si>
+  <si>
+    <t>Thrust Bearing Washer</t>
+  </si>
+  <si>
+    <t>5909K71</t>
+  </si>
+  <si>
+    <t>Propeller shaft attachment</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>8, 10, or 12 AWG wire</t>
+  </si>
+  <si>
+    <t>Epoxy or Acrylic glue</t>
+  </si>
+  <si>
+    <t>M4 X 10MM ?</t>
+  </si>
+  <si>
+    <t>mount gearbox</t>
+  </si>
+  <si>
+    <t>M3 X 10MM</t>
+  </si>
+  <si>
+    <t>oil seal cap</t>
+  </si>
+  <si>
+    <t>M4 X 25MM</t>
+  </si>
+  <si>
+    <t>nose cone to front cap</t>
+  </si>
+  <si>
+    <t>M5 X 25</t>
+  </si>
+  <si>
+    <t>nose cone foil mount</t>
+  </si>
+  <si>
+    <t>M5 NUT</t>
+  </si>
+  <si>
+    <t>MTS Parts</t>
+  </si>
+  <si>
+    <t>R101</t>
+  </si>
+  <si>
+    <t>motor tube</t>
+  </si>
+  <si>
+    <t>2.5IN OD 0.125IN WALL, 12IN Length 6061 T6 Tube</t>
+  </si>
+  <si>
+    <t>Online Metals, Mcmaster, Metal Supermarkets</t>
+  </si>
+  <si>
+    <t>R102</t>
+  </si>
+  <si>
+    <t>motor_gear_adapter_A</t>
+  </si>
+  <si>
+    <t>6061-T6 0.125IN</t>
+  </si>
+  <si>
+    <t>R103</t>
+  </si>
+  <si>
+    <t>motor_gear_adapter_B</t>
+  </si>
+  <si>
+    <t>R104</t>
+  </si>
+  <si>
+    <t>front_cap</t>
+  </si>
+  <si>
+    <t>6061-T6 2.5IN ROUND BAR</t>
+  </si>
+  <si>
+    <t>R105</t>
+  </si>
+  <si>
+    <t>gear_mount</t>
+  </si>
+  <si>
+    <t>R106</t>
+  </si>
+  <si>
+    <t>shaft_cap</t>
+  </si>
+  <si>
+    <t>R107</t>
+  </si>
+  <si>
+    <t>nose_cone_A</t>
+  </si>
+  <si>
+    <t>3D PRINT PLA</t>
+  </si>
+  <si>
+    <t>P108</t>
+  </si>
+  <si>
+    <t>nose_cone_B</t>
+  </si>
+  <si>
+    <t>R109</t>
+  </si>
+  <si>
+    <t>propeller</t>
+  </si>
+  <si>
+    <t>R110</t>
+  </si>
+  <si>
+    <t>reverse bushing</t>
+  </si>
+  <si>
+    <t>R111</t>
+  </si>
+  <si>
+    <t>Mast wire fairing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -392,22 +394,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -436,94 +423,67 @@
     </fill>
   </fills>
   <borders count="4">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -582,25 +542,320 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K36" activeCellId="0" sqref="K36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -648,7 +903,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -662,23 +917,23 @@
         <v>15</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="3">
         <v>160</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="3">
         <v>1.02</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -692,23 +947,23 @@
         <v>15</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="3">
         <v>150</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="3">
         <v>0.35</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -724,7 +979,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="n">
+      <c r="H5" s="3">
         <v>16</v>
       </c>
       <c r="I5" s="3"/>
@@ -732,7 +987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -746,11 +1001,11 @@
       <c r="E6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="3">
         <v>6.5</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3" t="n">
+      <c r="H6" s="3">
         <v>10</v>
       </c>
       <c r="I6" s="3"/>
@@ -758,7 +1013,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -774,13 +1029,13 @@
       <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="3">
         <v>13</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="3">
         <v>3</v>
       </c>
       <c r="I7" s="3"/>
@@ -788,7 +1043,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>34</v>
       </c>
@@ -802,19 +1057,19 @@
         <v>15</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="3">
         <v>150</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="3">
         <v>1</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -828,13 +1083,13 @@
         <v>40</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="3">
         <v>36</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="3">
         <v>1</v>
       </c>
       <c r="I9" s="3"/>
@@ -842,7 +1097,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -856,13 +1111,13 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="3">
         <v>2</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -876,19 +1131,19 @@
         <v>47</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="3">
         <v>60</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="3" t="n">
+      <c r="H11" s="3">
         <v>1</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
@@ -904,13 +1159,13 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3" t="n">
+      <c r="H12" s="3">
         <v>1</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -926,13 +1181,13 @@
       <c r="E13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="F13" s="3">
         <v>10</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="3" t="n">
+      <c r="H13" s="3">
         <v>1</v>
       </c>
       <c r="I13" s="3"/>
@@ -940,7 +1195,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>59</v>
       </c>
@@ -952,13 +1207,13 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3" t="n">
+      <c r="H14" s="3">
         <v>2</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>61</v>
       </c>
@@ -974,13 +1229,13 @@
       <c r="E15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="3" t="n">
+      <c r="F15" s="3">
         <v>12</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="3" t="n">
+      <c r="H15" s="3">
         <v>1</v>
       </c>
       <c r="I15" s="3"/>
@@ -988,7 +1243,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>64</v>
       </c>
@@ -1002,19 +1257,19 @@
       <c r="E16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="3">
         <v>3.7</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="3" t="n">
+      <c r="H16" s="3">
         <v>1</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>64</v>
       </c>
@@ -1030,13 +1285,13 @@
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="3" t="n">
+      <c r="H17" s="3">
         <v>2</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>69</v>
@@ -1048,13 +1303,13 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="3" t="n">
+      <c r="H18" s="3">
         <v>1</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>71</v>
@@ -1068,7 +1323,7 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>72</v>
@@ -1082,7 +1337,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>73</v>
@@ -1094,13 +1349,13 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
-      <c r="H21" s="3" t="n">
+      <c r="H21" s="3">
         <v>4</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>75</v>
@@ -1112,13 +1367,13 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3" t="n">
+      <c r="H22" s="3">
         <v>1</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>77</v>
@@ -1130,13 +1385,13 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="3" t="n">
+      <c r="H23" s="3">
         <v>4</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>79</v>
@@ -1148,13 +1403,13 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="3" t="n">
+      <c r="H24" s="3">
         <v>2</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>81</v>
@@ -1166,13 +1421,13 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="3" t="n">
+      <c r="H25" s="3">
         <v>2</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>82</v>
       </c>
@@ -1186,7 +1441,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>83</v>
       </c>
@@ -1200,21 +1455,21 @@
         <v>86</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="3" t="n">
+      <c r="F27" s="3">
         <v>20</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="3" t="n">
+      <c r="H27" s="3">
         <v>1</v>
       </c>
-      <c r="I27" s="3" t="n">
-        <v>0.325</v>
+      <c r="I27" s="3">
+        <v>0.32500000000000001</v>
       </c>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>87</v>
       </c>
@@ -1232,7 +1487,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>90</v>
       </c>
@@ -1250,7 +1505,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>92</v>
       </c>
@@ -1268,7 +1523,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>95</v>
       </c>
@@ -1286,7 +1541,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>97</v>
       </c>
@@ -1304,7 +1559,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>99</v>
       </c>
@@ -1322,7 +1577,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>102</v>
       </c>
@@ -1340,7 +1595,7 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>104</v>
       </c>
@@ -1358,7 +1613,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>106</v>
       </c>
@@ -1376,59 +1631,52 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>